<commit_message>
add input tests to make_changes_in_shifts
</commit_message>
<xml_diff>
--- a/workOnExcel/Constraints2.xlsx
+++ b/workOnExcel/Constraints2.xlsx
@@ -7,10 +7,73 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="shifts" sheetId="1" r:id="rId1"/>
+    <sheet name="adir" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="19">
+  <si>
+    <t>Sunday</t>
+  </si>
+  <si>
+    <t>Monday</t>
+  </si>
+  <si>
+    <t>Tuesday</t>
+  </si>
+  <si>
+    <t>Wednesday</t>
+  </si>
+  <si>
+    <t>Thursday</t>
+  </si>
+  <si>
+    <t>Friday</t>
+  </si>
+  <si>
+    <t>Saturday</t>
+  </si>
+  <si>
+    <t>Morning</t>
+  </si>
+  <si>
+    <t>adir</t>
+  </si>
+  <si>
+    <t>yoni</t>
+  </si>
+  <si>
+    <t>tair</t>
+  </si>
+  <si>
+    <t>asaf</t>
+  </si>
+  <si>
+    <t>rotem</t>
+  </si>
+  <si>
+    <t>stav</t>
+  </si>
+  <si>
+    <t>shift manager</t>
+  </si>
+  <si>
+    <t>emilia</t>
+  </si>
+  <si>
+    <t>michal</t>
+  </si>
+  <si>
+    <t>Evening</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -340,12 +403,226 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>